<commit_message>
Added Las file settings to the values being gathered from the excel Settings sheet
</commit_message>
<xml_diff>
--- a/lidar_settings.xlsx
+++ b/lidar_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\2019Host\neo\LiDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB68992-C117-4E31-AD80-B65D5BFA785F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B840E832-84AD-47FD-AE29-D3AC6C1D560C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25185" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{41D32DC6-A733-4811-B5BB-B5FA4829A855}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{41D32DC6-A733-4811-B5BB-B5FA4829A855}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
-  <si>
-    <t>Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>LiDAR settings</t>
   </si>
@@ -87,37 +84,6 @@
     <t>All times in nanoseconds</t>
   </si>
   <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6A9955"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>#How long to wait before deciding that all packets in a FOV has been recieved</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6A9955"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>#Dual mode = 2, single mode = 1. The programs understands the number of returns themself, this is used for testing</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> #Must be divisible by 60 and in the range [300, 1200], The LiDAR won't accept anything else. </t>
-  </si>
-  <si>
     <t>LiDAR lever arm</t>
   </si>
   <si>
@@ -134,31 +100,88 @@
   </si>
   <si>
     <t>The amount of leap seconds at the moment of flight can be found in the INS log file as "UTC offset"</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The spots containing the settings values have to be in the exact spot that they are at now (B6 -&gt; B25) </t>
+  </si>
+  <si>
+    <t>The names of the settings do not matter and can be changed to preference, now they have the names used in the lidar_values_and_settings.py file</t>
+  </si>
+  <si>
+    <t>To change their spot, you must also change the corresponding reference in lidar_values_and_settings.py</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Must be divisible by 60 and in the range [300, 1200], The LiDAR won't accept anything else. </t>
+  </si>
+  <si>
+    <t>Dual mode = 2, single mode = 1. The programs understands the number of returns themself, this is used for testing</t>
+  </si>
+  <si>
+    <t>How long to wait before deciding that all packets in a FOV has been recieved</t>
+  </si>
+  <si>
+    <t>So far I have used INS data boresight calibrated for the HySpex camera, so my lever arm is to the center of the HySpex camera</t>
+  </si>
+  <si>
+    <t>LAS file settings</t>
+  </si>
+  <si>
+    <t>scale x</t>
+  </si>
+  <si>
+    <t>scale y</t>
+  </si>
+  <si>
+    <t>scale z</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>max x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max y </t>
+  </si>
+  <si>
+    <t>max z</t>
+  </si>
+  <si>
+    <t>Our values are originally in mm, scale of 0.001 will convert them to meters</t>
+  </si>
+  <si>
+    <t>The limit before applying offset in mm, 1 million corresponds to 1 kilometer</t>
+  </si>
+  <si>
+    <t>Point format</t>
+  </si>
+  <si>
+    <t>The las point format you want to save the files in (1-10)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFD4D4D4"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF6A9955"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,14 +204,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5E462F-5D4E-489F-A29E-C545ED798189}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,173 +532,292 @@
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
       </c>
       <c r="B6">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>300</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <f>10^7</f>
+        <v>10000000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>10000000</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
       </c>
       <c r="B13">
         <v>2368</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>8308</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>-35.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>51.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>215.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>270</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>180</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>1E-3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <f>B33</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <f>B33</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <f>10^6</f>
+        <v>1000000</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <f>B37</f>
+        <v>1000000</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <f>B37</f>
+        <v>1000000</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the scale and offset value from the excel file to one more function, added some more descrition in the excel sheet
</commit_message>
<xml_diff>
--- a/lidar_settings.xlsx
+++ b/lidar_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\2019Host\neo\LiDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B840E832-84AD-47FD-AE29-D3AC6C1D560C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7073D893-FB9D-4571-806C-AF3A2E1329FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{41D32DC6-A733-4811-B5BB-B5FA4829A855}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>LiDAR settings</t>
   </si>
@@ -168,14 +168,23 @@
     <t>Point format</t>
   </si>
   <si>
-    <t>The las point format you want to save the files in (1-10)</t>
+    <t>Remember to save the Settings file before running the  python programs</t>
+  </si>
+  <si>
+    <t>The las point format you want to save the files in (1-10), you will currently get the same information whatever format you choose. And you will get an error if it's a format without the necessary fields like gps time</t>
+  </si>
+  <si>
+    <t>m/mm</t>
+  </si>
+  <si>
+    <t>r/min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,13 +192,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -201,13 +234,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -522,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5E462F-5D4E-489F-A29E-C545ED798189}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +590,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="S5" t="s">
@@ -581,8 +618,14 @@
       <c r="B7">
         <v>300</v>
       </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
       <c r="D7" t="s">
         <v>28</v>
+      </c>
+      <c r="S7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -612,7 +655,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -641,7 +684,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
@@ -718,7 +761,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -737,7 +780,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -749,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -759,6 +802,9 @@
       <c r="B33">
         <v>1E-3</v>
       </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
       <c r="D33" t="s">
         <v>42</v>
       </c>
@@ -771,6 +817,9 @@
         <f>B33</f>
         <v>1E-3</v>
       </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -780,6 +829,9 @@
         <f>B33</f>
         <v>1E-3</v>
       </c>
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -822,6 +874,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added the file paths in the excel Settings, so that you dont have to manually choose them if you dont want to, if left empty you will be promptet
</commit_message>
<xml_diff>
--- a/lidar_settings.xlsx
+++ b/lidar_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\2019Host\neo\LiDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7073D893-FB9D-4571-806C-AF3A2E1329FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B85400E-8D88-459D-B0A6-CBA978F3CAC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{41D32DC6-A733-4811-B5BB-B5FA4829A855}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>LiDAR settings</t>
   </si>
@@ -132,9 +132,6 @@
     <t>LAS file settings</t>
   </si>
   <si>
-    <t>scale x</t>
-  </si>
-  <si>
     <t>scale y</t>
   </si>
   <si>
@@ -178,13 +175,113 @@
   </si>
   <si>
     <t>r/min</t>
+  </si>
+  <si>
+    <t>num_frames</t>
+  </si>
+  <si>
+    <t>scale_x</t>
+  </si>
+  <si>
+    <t>read_pcap_from_file.py settings:</t>
+  </si>
+  <si>
+    <t>lidar_values_and_settings.py settings:</t>
+  </si>
+  <si>
+    <t>From pcap</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">number of frames to be created from the pcap (it will read in the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>first</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> n files</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>num_frames_per_las_file</t>
+  </si>
+  <si>
+    <t>packet_devisor</t>
+  </si>
+  <si>
+    <t>For quick analysis you can choose to skip every n packet from being processed</t>
+  </si>
+  <si>
+    <t>From frame files</t>
+  </si>
+  <si>
+    <t>temp_location_frame_files</t>
+  </si>
+  <si>
+    <t>./files_from_pcap/</t>
+  </si>
+  <si>
+    <t>The location for saving the las files containing only one frame each</t>
+  </si>
+  <si>
+    <t>The amount of frames to load and put together in one las file, keep in mind that this amount must be stored in memory</t>
+  </si>
+  <si>
+    <t>flight_scans</t>
+  </si>
+  <si>
+    <t>flight_ins</t>
+  </si>
+  <si>
+    <t>outfile_directory</t>
+  </si>
+  <si>
+    <t>./flight_scans/wireshark_flight_1.pcap</t>
+  </si>
+  <si>
+    <t>./flight_ins/export_flight01_20.08.19_all.txt</t>
+  </si>
+  <si>
+    <t>./processed_las/garbage/</t>
+  </si>
+  <si>
+    <t>The path fields accept relative and absolute paths, but only in unix syntax</t>
+  </si>
+  <si>
+    <t>If the path fields are left empty, or the path dir or file doesn't exist, the program will prompt you for manual selection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +298,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -557,16 +662,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5E462F-5D4E-489F-A29E-C545ED798189}">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -585,6 +690,9 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
       <c r="S4" t="s">
         <v>26</v>
       </c>
@@ -605,7 +713,7 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S6" t="s">
         <v>16</v>
@@ -619,13 +727,13 @@
         <v>300</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -638,6 +746,9 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
+      <c r="S8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -702,7 +813,7 @@
         <v>-35.5</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,7 +824,7 @@
         <v>51.9</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -724,7 +835,7 @@
         <v>215.7</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,7 +846,7 @@
         <v>270</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,7 +857,7 @@
         <v>180</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -773,12 +884,15 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
@@ -786,90 +900,180 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>1E-3</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <f>B33</f>
         <v>1E-3</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <f>B33</f>
         <v>1E-3</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <f>10^6</f>
         <v>1000000</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <f>B37</f>
         <v>1000000</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <f>B37</f>
         <v>1000000</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>200</v>
+      </c>
+      <c r="D52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f>B51*200</f>
+        <v>200</v>
+      </c>
+      <c r="D55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the system so that the original frame_files are deleted after being stored in the new collected las file. This is in preperation of being able to do the process in two steps and so that the files are not lost during an error
</commit_message>
<xml_diff>
--- a/lidar_settings.xlsx
+++ b/lidar_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\2019Host\neo\LiDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B85400E-8D88-459D-B0A6-CBA978F3CAC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D376A3B-6034-43F3-9575-18D4DCB0512C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{41D32DC6-A733-4811-B5BB-B5FA4829A855}"/>
   </bookViews>
@@ -665,7 +665,7 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Last working version before going down to NEO, added the options to only process from pcap to frame files, and the option to only collect frame files. Also added the option to choose between seperation on lasers and collecting everything.
</commit_message>
<xml_diff>
--- a/lidar_settings.xlsx
+++ b/lidar_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\2019Host\neo\LiDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D376A3B-6034-43F3-9575-18D4DCB0512C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E29C89-DF9B-4731-AC2A-4E6E91DE13D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{41D32DC6-A733-4811-B5BB-B5FA4829A855}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>LiDAR settings</t>
   </si>
@@ -268,13 +268,31 @@
     <t>./flight_ins/export_flight01_20.08.19_all.txt</t>
   </si>
   <si>
-    <t>./processed_las/garbage/</t>
-  </si>
-  <si>
     <t>The path fields accept relative and absolute paths, but only in unix syntax</t>
   </si>
   <si>
     <t>If the path fields are left empty, or the path dir or file doesn't exist, the program will prompt you for manual selection</t>
+  </si>
+  <si>
+    <t>./processed_las/rotation_matrix_from_excel/</t>
+  </si>
+  <si>
+    <t>Rotates yaw first</t>
+  </si>
+  <si>
+    <t>Pitch secondly</t>
+  </si>
+  <si>
+    <t>Roll third</t>
+  </si>
+  <si>
+    <t>If this value is 1, files in the temp_location_frame_files will be processed. Set to 0 to not run</t>
+  </si>
+  <si>
+    <t>If this value is 1, PCAP files will be processed into frame_files. Set to 0 to not run</t>
+  </si>
+  <si>
+    <t>Separate files on laser id</t>
   </si>
 </sst>
 </file>
@@ -662,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5E462F-5D4E-489F-A29E-C545ED798189}">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +765,7 @@
         <v>29</v>
       </c>
       <c r="S8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -843,10 +861,13 @@
         <v>12</v>
       </c>
       <c r="B20">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
         <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,6 +880,9 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -869,6 +893,9 @@
       </c>
       <c r="C22" t="s">
         <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,7 +936,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -923,7 +950,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -935,7 +962,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -947,7 +974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -962,7 +989,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -974,7 +1001,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -986,31 +1013,37 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
       <c r="D46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
       <c r="B47" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -1018,7 +1051,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -1029,7 +1062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1040,7 +1073,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -1051,12 +1084,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1068,12 +1107,20 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>64</v>
       </c>
-      <c r="B56" t="s">
-        <v>67</v>
+      <c r="E56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>